<commit_message>
Dec 17, 2017 8:50pm
</commit_message>
<xml_diff>
--- a/inst/extdata/test_size_data.xlsx
+++ b/inst/extdata/test_size_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michael/Documents/Programing_R/test_folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michael/Documents/Programing_R/AntBite_1.0/AntBite/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19520" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>individual</t>
   </si>
@@ -44,25 +44,79 @@
     <t>mandi_length</t>
   </si>
   <si>
-    <t>sp_01_01</t>
-  </si>
-  <si>
-    <t>sp_01_02</t>
-  </si>
-  <si>
-    <t>sp_02_01</t>
-  </si>
-  <si>
-    <t>sp_02_02</t>
-  </si>
-  <si>
-    <t>Sp_1</t>
-  </si>
-  <si>
-    <t>Sp_2</t>
-  </si>
-  <si>
-    <t>Sp_3</t>
+    <t>mdr_039_01</t>
+  </si>
+  <si>
+    <t>mdr_039_02</t>
+  </si>
+  <si>
+    <t>mdr_039_03</t>
+  </si>
+  <si>
+    <t>mdr_039_04</t>
+  </si>
+  <si>
+    <t>mdr_039_05</t>
+  </si>
+  <si>
+    <t>mdr_039_06</t>
+  </si>
+  <si>
+    <t>mdr_039_07</t>
+  </si>
+  <si>
+    <t>mdr_039_08</t>
+  </si>
+  <si>
+    <t>mdr_039_09</t>
+  </si>
+  <si>
+    <t>mdr_039_10</t>
+  </si>
+  <si>
+    <t>Atta</t>
+  </si>
+  <si>
+    <t>mdr_046_01</t>
+  </si>
+  <si>
+    <t>mdr_046_02</t>
+  </si>
+  <si>
+    <t>mdr_046_04</t>
+  </si>
+  <si>
+    <t>mdr_046_05</t>
+  </si>
+  <si>
+    <t>mdr_046_06</t>
+  </si>
+  <si>
+    <t>mdr_046_07</t>
+  </si>
+  <si>
+    <t>mdr_046_08</t>
+  </si>
+  <si>
+    <t>Pheidole</t>
+  </si>
+  <si>
+    <t>rpn_005_02</t>
+  </si>
+  <si>
+    <t>rpn_005_03</t>
+  </si>
+  <si>
+    <t>rpn_005_04</t>
+  </si>
+  <si>
+    <t>rpn_005_05</t>
+  </si>
+  <si>
+    <t>rpn_005_06</t>
+  </si>
+  <si>
+    <t>Plectroctena</t>
   </si>
 </sst>
 </file>
@@ -377,13 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -407,18 +464,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>2.2400000000000002</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D2">
-        <f>C2*1.3</f>
-        <v>2.9120000000000004</v>
+        <v>2.1</v>
       </c>
       <c r="E2">
-        <f>D2*0.6</f>
-        <v>1.7472000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -426,18 +481,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>2.67</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">C3*1.3</f>
-        <v>3.4710000000000001</v>
+        <v>2.13</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E5" si="1">D3*0.6</f>
-        <v>2.0825999999999998</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -445,18 +498,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>3.46</v>
+        <v>2.42</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>4.4980000000000002</v>
+        <v>2.02</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
-        <v>2.6987999999999999</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -464,37 +515,322 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>4.46</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>5.798</v>
+        <v>1.89</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
-        <v>3.4788000000000001</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>2.33</v>
+      </c>
+      <c r="D6">
+        <v>1.89</v>
+      </c>
+      <c r="E6">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>2.52</v>
+      </c>
+      <c r="D7">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E7">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ref="D6" si="2">C6*1.3</f>
-        <v>6.3180000000000005</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6" si="3">D6*0.6</f>
-        <v>3.7907999999999999</v>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E8">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>3.53</v>
+      </c>
+      <c r="D9">
+        <v>2.87</v>
+      </c>
+      <c r="E9">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D10">
+        <v>1.92</v>
+      </c>
+      <c r="E10">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>2.5</v>
+      </c>
+      <c r="D11">
+        <v>2.1</v>
+      </c>
+      <c r="E11">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>1.93</v>
+      </c>
+      <c r="D12">
+        <v>1.59</v>
+      </c>
+      <c r="E12">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>1.99</v>
+      </c>
+      <c r="D13">
+        <v>1.64</v>
+      </c>
+      <c r="E13">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>1.86</v>
+      </c>
+      <c r="D14">
+        <v>1.42</v>
+      </c>
+      <c r="E14">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>1.96</v>
+      </c>
+      <c r="D15">
+        <v>1.67</v>
+      </c>
+      <c r="E15">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D16">
+        <v>1.65</v>
+      </c>
+      <c r="E16">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>1.95</v>
+      </c>
+      <c r="D17">
+        <v>1.65</v>
+      </c>
+      <c r="E17">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D18">
+        <v>1.75</v>
+      </c>
+      <c r="E18">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <v>3.33</v>
+      </c>
+      <c r="D19">
+        <v>3.46</v>
+      </c>
+      <c r="E19">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>3.59</v>
+      </c>
+      <c r="D20">
+        <v>3.69</v>
+      </c>
+      <c r="E20">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>3.51</v>
+      </c>
+      <c r="D21">
+        <v>3.63</v>
+      </c>
+      <c r="E21">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>3.54</v>
+      </c>
+      <c r="D22">
+        <v>3.72</v>
+      </c>
+      <c r="E22">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>3.37</v>
+      </c>
+      <c r="D23">
+        <v>3.6</v>
+      </c>
+      <c r="E23">
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>